<commit_message>
Update in scripts 07/20
</commit_message>
<xml_diff>
--- a/Test Data/Policy Number_RO.xlsx
+++ b/Test Data/Policy Number_RO.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asllie Sablan\Katalon Studio\GIT\SN-RO_Repo\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93018EA6-FCF6-4217-93F0-531CBC7E370A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{93018EA6-FCF6-4217-93F0-531CBC7E370A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BBBB5CE8-4498-4642-A532-4F55D86E2EBB}"/>
+    <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{BBBB5CE8-4498-4642-A532-4F55D86E2EBB}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="AL_Policy Number" sheetId="4" r:id="rId1"/>
-    <sheet name="APD_Policy Number" sheetId="5" r:id="rId2"/>
+    <sheet name="AL_Policy Number" r:id="rId1" sheetId="4"/>
+    <sheet name="APD_Policy Number" r:id="rId2" sheetId="5"/>
   </sheets>
   <definedNames>
     <definedName name="Business_Type_Code">#REF!</definedName>
@@ -60,7 +60,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -76,18 +76,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Auto Liability Policy Number</t>
   </si>
   <si>
     <t>Auto Physical Damage Policy Number</t>
+  </si>
+  <si>
+    <t>TUN-OR-0001112</t>
+  </si>
+  <si>
+    <t>TUN-OR-0001113</t>
+  </si>
+  <si>
+    <t>TUO-OR-0001620</t>
+  </si>
+  <si>
+    <t>TUN-MT-0001115</t>
+  </si>
+  <si>
+    <t>TUO-MT-0001622</t>
+  </si>
+  <si>
+    <t>TUN-CA-0001117</t>
+  </si>
+  <si>
+    <t>TUO-CA-0001623</t>
+  </si>
+  <si>
+    <t>TUN-IL-0001118</t>
+  </si>
+  <si>
+    <t>TUO-IL-0001624</t>
+  </si>
+  <si>
+    <t>TUN-IL-0001122</t>
+  </si>
+  <si>
+    <t>TUN-IL-0001123</t>
+  </si>
+  <si>
+    <t>TUO-IL-0001625</t>
+  </si>
+  <si>
+    <t>TUN-IL-0001128</t>
+  </si>
+  <si>
+    <t>TUN-IL-0001129</t>
+  </si>
+  <si>
+    <t>TUN-IL-0001130</t>
+  </si>
+  <si>
+    <t>TUO-IL-0001629</t>
+  </si>
+  <si>
+    <t>TUN-MT-0001172</t>
+  </si>
+  <si>
+    <t>TUO-MT-0001639</t>
+  </si>
+  <si>
+    <t>TUN-MT-0001174</t>
+  </si>
+  <si>
+    <t>TUO-MT-0001640</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -129,19 +190,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -165,7 +226,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -182,10 +243,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -220,7 +281,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -272,7 +333,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -383,21 +444,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -414,7 +475,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -466,25 +527,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0BEA5C-56BD-409B-85F3-7104E1C06770}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0BEA5C-56BD-409B-85F3-7104E1C06770}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -492,28 +553,88 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule dxfId="1" priority="2" type="duplicateValues"/>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72EF98E-B9FC-462A-96D9-DA123632D0C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72EF98E-B9FC-462A-96D9-DA123632D0C9}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -521,10 +642,50 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule dxfId="0" priority="1" type="duplicateValues"/>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>